<commit_message>
black & moved unused files to new branch
</commit_message>
<xml_diff>
--- a/streamlit/templates/Address_template_split.xlsx
+++ b/streamlit/templates/Address_template_split.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul.carroll/Github/pycom/nhs_time_of_travel/streamlit/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D053597-3F36-C94F-B1C3-68F39F6474BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD421261-1CF5-7049-8ADB-B0292925ADE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="68040" yWindow="780" windowWidth="29580" windowHeight="17180" xr2:uid="{EF08C01F-1A25-6E46-B3B0-470DDF1A58B3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Ipswich Hospital</t>
   </si>
   <si>
-    <t xml:space="preserve">St Clements Hospital </t>
-  </si>
-  <si>
     <t>Walker Close</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
   </si>
   <si>
     <t>3 Walker Close, Ipswich, Suffolk, IP3 8LS</t>
-  </si>
-  <si>
-    <t>Foxhall Road, Ipswich, Suffolk, IP4 5PF</t>
   </si>
   <si>
     <t>25 Sheerwater way</t>
@@ -438,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130D6FBD-61C5-0145-B4F6-07535D218775}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,10 +454,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -471,7 +465,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -479,7 +473,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -487,7 +481,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -496,14 +490,6 @@
       </c>
       <c r="B6" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>